<commit_message>
more updates to backtest and reporting
</commit_message>
<xml_diff>
--- a/PresentationTop20-2026-01-08_fmp_stock_NA1_EU1.xlsx
+++ b/PresentationTop20-2026-01-08_fmp_stock_NA1_EU1.xlsx
@@ -23,9 +23,9 @@
     <sheet name="HSM.L" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="RRBI" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="NEXN" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="0HQ7.L" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="BKE" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="M12.DE" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="M12.DE" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="0HQ7.L" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="BKE" sheetId="19" state="visible" r:id="rId19"/>
     <sheet name="GFM.L" sheetId="20" state="visible" r:id="rId20"/>
     <sheet name="Sheet" sheetId="21" state="visible" r:id="rId21"/>
   </sheets>
@@ -625,7 +625,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>4,050.62 million</t>
+          <t>4,087.95 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -1154,12 +1154,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1410.0000</t>
+          <t>1380.0000</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0.0164</t>
+          <t>0.0168</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -1174,7 +1174,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>548.27 million</t>
+          <t>544.33 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -1464,7 +1464,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>2.1053</t>
+          <t>2.151</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>652.71 million</t>
+          <t>644.88 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -2242,12 +2242,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>5.3300</t>
+          <t>5.3100</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0.6884</t>
+          <t>0.6910</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -2262,7 +2262,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>7,202.06 million</t>
+          <t>7,134.50 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -2552,7 +2552,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>2.4963</t>
+          <t>2.5056</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -3869,12 +3869,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>71.3800</t>
+          <t>72.8100</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>1.0079</t>
+          <t>0.9881</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -3889,7 +3889,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>480.55 million</t>
+          <t>490.92 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -4179,7 +4179,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>1.699</t>
+          <t>1.6813</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -4428,7 +4428,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>181.15 million</t>
+          <t>181.45 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -4833,7 +4833,7 @@
     <col width="21" customWidth="1" min="12" max="12"/>
     <col width="6" customWidth="1" min="13" max="13"/>
     <col width="19" customWidth="1" min="14" max="14"/>
-    <col width="17" customWidth="1" min="15" max="15"/>
+    <col width="25" customWidth="1" min="15" max="15"/>
     <col width="23" customWidth="1" min="16" max="16"/>
   </cols>
   <sheetData>
@@ -4917,72 +4917,72 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>0HQ7.L</t>
+          <t>M12.DE</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-02-01</t>
+          <t>2024-12-31</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>8.2240</t>
+          <t>5.2005</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>12.1595</t>
+          <t>19.2288</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>5.6082</t>
+          <t>2.9030</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2.0530</t>
+          <t>1.9096</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>8.3314</t>
+          <t>3.0225</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>5.6082</t>
+          <t>2.9030</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>53.8900</t>
+          <t>18.6000</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0.5075</t>
+          <t>0.5666</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>The Buckle, Inc.</t>
+          <t>M1 Kliniken AG</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>1.0310</t>
+          <t>1.0370</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2,731.31 million</t>
+          <t>349.28 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Apparel - Retail</t>
+          <t>Medical - Care Facilities</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -4994,42 +4994,42 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>0HQ7.L</t>
+          <t>M12.DE</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-02-03</t>
+          <t>2023-12-31</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>11.6784</t>
+          <t>4.7964</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>8.5628</t>
+          <t>20.8492</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>4.5572</t>
+          <t>1.8915</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2.0061</t>
+          <t>1.8986</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>10.4474</t>
+          <t>0.9247</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>4.5572</t>
+          <t>1.8915</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -5042,49 +5042,49 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Consumer Cyclical</t>
+          <t>Healthcare</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>0HQ7.L</t>
+          <t>M12.DE</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2023-01-28</t>
+          <t>2022-12-31</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>11.9217</t>
+          <t>2.6018</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>8.3880</t>
+          <t>38.4342</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>5.6756</t>
+          <t>1.7372</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1.8728</t>
+          <t>2.8641</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>9.4988</t>
+          <t>1.0989</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>5.6756</t>
+          <t>1.7372</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -5099,42 +5099,42 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>0HQ7.L</t>
+          <t>M12.DE</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2022-01-29</t>
+          <t>2021-12-31</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>14.2416</t>
+          <t>6.3905</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>7.0217</t>
+          <t>15.6482</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>5.7179</t>
+          <t>1.4664</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1.5740</t>
+          <t>2.5380</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>19.4381</t>
+          <t>1.1896</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>5.7179</t>
+          <t>1.4664</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -5149,42 +5149,42 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>0HQ7.L</t>
+          <t>M12.DE</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2021-01-30</t>
+          <t>2020-12-31</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>6.7885</t>
+          <t>3.9735</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>14.7308</t>
+          <t>25.1664</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>4.8333</t>
+          <t>2.0024</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2.1188</t>
+          <t>2.1079</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>6.7009</t>
+          <t>0.0748</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>4.8333</t>
+          <t>2.0024</t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -5214,42 +5214,42 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>0HQ7.L</t>
+          <t>M12.DE</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2020-02-01</t>
+          <t>2019-12-31</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>8.8051</t>
+          <t>3.8877</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>11.3571</t>
+          <t>25.7220</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>3.0477</t>
+          <t>3.6682</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2.1943</t>
+          <t>4.1104</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>9.5154</t>
+          <t>2.0979</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>3.0477</t>
+          <t>3.6682</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -5267,75 +5267,75 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>1.6824</t>
+          <t>2.5298</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>0H9G.L</t>
+          <t>SBS.DE</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="P8" t="inlineStr">
         <is>
-          <t>0J2X.L</t>
+          <t>NP5.DE</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="P9" t="inlineStr">
         <is>
-          <t>0R2I.L</t>
+          <t>ILM1.DE</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="P10" t="inlineStr">
         <is>
-          <t>0ZFN.L</t>
+          <t>MED.DE</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="P11" t="inlineStr">
         <is>
-          <t>0KJQ.L</t>
+          <t>2LYA.F</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="P12" t="inlineStr">
         <is>
-          <t>0KTF.L</t>
+          <t>LIK.DE</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="P13" t="inlineStr">
         <is>
-          <t>0KEQ.L</t>
+          <t>94E.F</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="P14" t="inlineStr">
         <is>
-          <t>0R32.L</t>
+          <t>FYB.DE</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="P15" t="inlineStr">
         <is>
-          <t>0QYY.L</t>
+          <t>V3V.DE</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="P16" t="inlineStr">
         <is>
-          <t>0LWH.L</t>
+          <t>UOM.MU</t>
         </is>
       </c>
     </row>
@@ -5456,7 +5456,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>BKE</t>
+          <t>0HQ7.L</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -5496,12 +5496,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>53.8900</t>
+          <t>55.3500</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0.5075</t>
+          <t>0.4941</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -5516,7 +5516,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2,756.83 million</t>
+          <t>2,780.70 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -5533,7 +5533,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>BKE</t>
+          <t>0HQ7.L</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -5588,7 +5588,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>BKE</t>
+          <t>0HQ7.L</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -5638,7 +5638,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>BKE</t>
+          <t>0HQ7.L</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -5688,7 +5688,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>BKE</t>
+          <t>0HQ7.L</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -5753,7 +5753,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>BKE</t>
+          <t>0HQ7.L</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -5806,75 +5806,75 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>1.6824</t>
+          <t>1.6346</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>AEO</t>
+          <t>0H9G.L</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="P8" t="inlineStr">
         <is>
-          <t>VSCO</t>
+          <t>0J2X.L</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="P9" t="inlineStr">
         <is>
-          <t>COLM</t>
+          <t>0R2I.L</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="P10" t="inlineStr">
         <is>
-          <t>ANF</t>
+          <t>0ZFN.L</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="P11" t="inlineStr">
         <is>
-          <t>GEF</t>
+          <t>0KJQ.L</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="P12" t="inlineStr">
         <is>
-          <t>AAP</t>
+          <t>0KTF.L</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="P13" t="inlineStr">
         <is>
-          <t>YETI</t>
+          <t>0KEQ.L</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="P14" t="inlineStr">
         <is>
-          <t>VC</t>
+          <t>0R32.L</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="P15" t="inlineStr">
         <is>
-          <t>PRKS</t>
+          <t>0QYY.L</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="P16" t="inlineStr">
         <is>
-          <t>GRBK</t>
+          <t>0LWH.L</t>
         </is>
       </c>
     </row>
@@ -5911,7 +5911,7 @@
     <col width="21" customWidth="1" min="12" max="12"/>
     <col width="6" customWidth="1" min="13" max="13"/>
     <col width="19" customWidth="1" min="14" max="14"/>
-    <col width="25" customWidth="1" min="15" max="15"/>
+    <col width="17" customWidth="1" min="15" max="15"/>
     <col width="23" customWidth="1" min="16" max="16"/>
   </cols>
   <sheetData>
@@ -5995,72 +5995,72 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>M12.DE</t>
+          <t>BKE</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-12-31</t>
+          <t>2025-02-01</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>5.2005</t>
+          <t>8.2240</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>19.2288</t>
+          <t>12.1595</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2.9030</t>
+          <t>5.6082</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1.9096</t>
+          <t>2.0530</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>3.0225</t>
+          <t>8.3314</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2.9030</t>
+          <t>5.6082</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>18.7000</t>
+          <t>55.3500</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0.5636</t>
+          <t>0.4941</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>M1 Kliniken AG</t>
+          <t>The Buckle, Inc.</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>1.0370</t>
+          <t>1.0310</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>351.90 million</t>
+          <t>2,848.40 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Medical - Care Facilities</t>
+          <t>Apparel - Retail</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -6072,42 +6072,42 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>M12.DE</t>
+          <t>BKE</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2023-12-31</t>
+          <t>2024-02-03</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>4.7964</t>
+          <t>11.6784</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>20.8492</t>
+          <t>8.5628</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1.8915</t>
+          <t>4.5572</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1.8986</t>
+          <t>2.0061</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.9247</t>
+          <t>10.4474</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>1.8915</t>
+          <t>4.5572</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -6120,49 +6120,49 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Healthcare</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>M12.DE</t>
+          <t>BKE</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2022-12-31</t>
+          <t>2023-01-28</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2.6018</t>
+          <t>11.9217</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>38.4342</t>
+          <t>8.3880</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.7372</t>
+          <t>5.6756</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2.8641</t>
+          <t>1.8728</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>1.0989</t>
+          <t>9.4988</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>1.7372</t>
+          <t>5.6756</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -6177,42 +6177,42 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>M12.DE</t>
+          <t>BKE</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2021-12-31</t>
+          <t>2022-01-29</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>6.3905</t>
+          <t>14.2416</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>15.6482</t>
+          <t>7.0217</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.4664</t>
+          <t>5.7179</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2.5380</t>
+          <t>1.5740</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>1.1896</t>
+          <t>19.4381</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>1.4664</t>
+          <t>5.7179</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -6227,42 +6227,42 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>M12.DE</t>
+          <t>BKE</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2020-12-31</t>
+          <t>2021-01-30</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>3.9735</t>
+          <t>6.7885</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>25.1664</t>
+          <t>14.7308</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2.0024</t>
+          <t>4.8333</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2.1079</t>
+          <t>2.1188</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0.0748</t>
+          <t>6.7009</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2.0024</t>
+          <t>4.8333</t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -6292,42 +6292,42 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>M12.DE</t>
+          <t>BKE</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2019-12-31</t>
+          <t>2020-02-01</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>3.8877</t>
+          <t>8.8051</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>25.7220</t>
+          <t>11.3571</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>3.6682</t>
+          <t>3.0477</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>4.1104</t>
+          <t>2.1943</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2.0979</t>
+          <t>9.5154</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>3.6682</t>
+          <t>3.0477</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -6345,75 +6345,75 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>2.5165</t>
+          <t>1.6346</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>SBS.DE</t>
+          <t>AEO</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="P8" t="inlineStr">
         <is>
-          <t>NP5.DE</t>
+          <t>VSCO</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="P9" t="inlineStr">
         <is>
-          <t>ILM1.DE</t>
+          <t>COLM</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="P10" t="inlineStr">
         <is>
-          <t>MED.DE</t>
+          <t>ANF</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="P11" t="inlineStr">
         <is>
-          <t>2LYA.F</t>
+          <t>GEF</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="P12" t="inlineStr">
         <is>
-          <t>LIK.DE</t>
+          <t>AAP</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="P13" t="inlineStr">
         <is>
-          <t>94E.F</t>
+          <t>YETI</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="P14" t="inlineStr">
         <is>
-          <t>FYB.DE</t>
+          <t>VC</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="P15" t="inlineStr">
         <is>
-          <t>V3V.DE</t>
+          <t>PRKS</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="P16" t="inlineStr">
         <is>
-          <t>UOM.MU</t>
+          <t>GRBK</t>
         </is>
       </c>
     </row>
@@ -6594,7 +6594,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>278.87 million</t>
+          <t>280.95 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -7133,7 +7133,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>479.89 million</t>
+          <t>479.08 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -7670,12 +7670,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>36.3200</t>
+          <t>35.9800</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2.6604</t>
+          <t>2.6855</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -7690,7 +7690,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>938.23 million</t>
+          <t>940.38 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -7980,7 +7980,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>1.3719</t>
+          <t>1.3861</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -8188,12 +8188,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>36.3200</t>
+          <t>35.9800</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2.6604</t>
+          <t>2.6855</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -8208,7 +8208,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>1,299.19 million</t>
+          <t>1,283.45 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -8498,7 +8498,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>1.3719</t>
+          <t>1.3861</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -8726,7 +8726,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>57.11 million</t>
+          <t>56.53 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -9275,7 +9275,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>227.61 million</t>
+          <t>231.54 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -9824,7 +9824,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>33,157.53 million</t>
+          <t>33,286.47 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -10366,7 +10366,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>7,565.97 million</t>
+          <t>7,573.55 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -10895,12 +10895,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>395.0000</t>
+          <t>388.0000</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0.0080</t>
+          <t>0.0081</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -10915,7 +10915,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>127.48 million</t>
+          <t>125.54 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -11205,7 +11205,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>2.0993</t>
+          <t>2.1386</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">

</xml_diff>

<commit_message>
updated backtestinga nd reporting
</commit_message>
<xml_diff>
--- a/PresentationTop20-2026-01-08_fmp_stock_NA1_EU1.xlsx
+++ b/PresentationTop20-2026-01-08_fmp_stock_NA1_EU1.xlsx
@@ -625,7 +625,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>4,087.95 million</t>
+          <t>4,088.57 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -2262,7 +2262,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>7,134.50 million</t>
+          <t>7,175.03 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -3889,7 +3889,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>490.92 million</t>
+          <t>492.67 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -4428,7 +4428,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>181.45 million</t>
+          <t>180.22 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -6055,7 +6055,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2,848.40 million</t>
+          <t>2,844.82 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -8208,7 +8208,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>1,283.45 million</t>
+          <t>1,287.03 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -9824,7 +9824,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>33,286.47 million</t>
+          <t>33,271.30 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -10366,7 +10366,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>7,573.55 million</t>
+          <t>7,565.97 million</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">

</xml_diff>